<commit_message>
schedule, issue file add
</commit_message>
<xml_diff>
--- a/일정_서승현.xlsx
+++ b/일정_서승현.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>11월</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,19 +77,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Map Terrain 텍스쳐 깨짐현상 해결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Map Resources Test (X파일 사용결정)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Map Resources List 작성 후 Map 만들기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map object BoundingBox 처리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">조원들과 Map feedBack 하기 </t>
+    <t>Map Resources Test (X파일 리스트 테스트)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map 위에 오브젝트올리기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오브젝트들 Alpha 현상 해결중..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>terrainMap.X와 surfaceMap.X 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map 크기와 갯수 캐릭터와 조절 및 결정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map위에 오브젝트 올려서 크기 및 위치결정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map 리소스추출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map 피드백</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -101,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +191,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +263,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -450,7 +495,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -550,6 +595,39 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -574,22 +652,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -872,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:AK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -906,13 +990,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="19"/>
       <c r="G1" s="27"/>
       <c r="H1" s="19" t="s">
@@ -951,11 +1035,11 @@
       <c r="AK1" s="21"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="19"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -992,11 +1076,11 @@
       <c r="AK2" s="21"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="19"/>
       <c r="G3" s="23"/>
       <c r="H3" s="19"/>
@@ -1031,47 +1115,47 @@
       <c r="AK3" s="21"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="33" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="34" t="s">
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="45"/>
+      <c r="AB4" s="45"/>
+      <c r="AC4" s="45"/>
+      <c r="AD4" s="45"/>
+      <c r="AE4" s="45"/>
+      <c r="AF4" s="45"/>
+      <c r="AG4" s="45"/>
+      <c r="AH4" s="45"/>
+      <c r="AI4" s="45"/>
+      <c r="AJ4" s="45"/>
+      <c r="AK4" s="45"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1191,65 +1275,160 @@
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
+        <v>22</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="43"/>
       <c r="AK6" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="E7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="25"/>
+        <v>23</v>
+      </c>
+      <c r="F7" s="52"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="43"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F8" s="29"/>
       <c r="G8" s="30"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="41"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
       <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="E9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="31"/>
+        <v>15</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
       <c r="I9" s="32"/>
       <c r="J9" s="30"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
       <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="E10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E11" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="30"/>
-      <c r="M10" s="41"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
+      <c r="V13" s="57"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="34"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="41"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="41"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="E16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="59"/>
+    </row>
+    <row r="17" spans="19:22" x14ac:dyDescent="0.3">
+      <c r="S17" s="58"/>
+      <c r="T17" s="59"/>
+    </row>
+    <row r="18" spans="19:22" x14ac:dyDescent="0.3">
+      <c r="U18" s="30"/>
+      <c r="V18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>